<commit_message>
updated prompt, removed rouge-2 and rouge-l
</commit_message>
<xml_diff>
--- a/results/config.xlsx
+++ b/results/config.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -464,7 +464,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -519,7 +519,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>You are an advanced anonymizer that replaces personally identifiable information (PII) with a category label. You will NOT paraphrase or change any part of the text except for replacing PII with its category in square brackets.
+          <t>You are an advanced anonymizer that replaces personally identifiable information (PII) with a category label. You will replacing PII with its category in square brackets.
 Example:
 Input: My name is Alice and I live in London.
 Output: My name is [NAME] and I live in [LOCATION].</t>

</xml_diff>

<commit_message>
add run 5000 data point results
</commit_message>
<xml_diff>
--- a/results/config.xlsx
+++ b/results/config.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[0.001, 0.5, 1.0]</t>
+          <t>[0.001, 0.1, 0.2, 0.3, 0.4, 0.5, 0.6, 0.7, 0.8, 0.9, 1.0]</t>
         </is>
       </c>
     </row>
@@ -464,7 +464,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>50</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="4">
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>50</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="5">
@@ -519,7 +519,9 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>You are an advanced anonymizer that replaces personally identifiable information (PII) with a category label. You will NOT paraphrase or change any part of the text except for replacing PII with its category in square brackets.
+          <t>You are an advanced anonymiser that replaces personally identifiable information (PII) with a category label. Your task is to:
+1) Replace PII with its category in square brackets
+2) Preserve the context and utility of the original input
 Example:
 Input: My name is Alice and I live in London.
 Output: My name is [NAME] and I live in [LOCATION].</t>
@@ -544,7 +546,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>sys.version_info(major=3, minor=10, micro=11, releaselevel='final', serial=0)</t>
+          <t>sys.version_info(major=3, minor=10, micro=12, releaselevel='final', serial=0)</t>
         </is>
       </c>
     </row>

</xml_diff>